<commit_message>
New developments with 100000 pupolation
</commit_message>
<xml_diff>
--- a/data/states.xlsx
+++ b/data/states.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tumelos_sun_ac_za/Documents/Documents/SACEMAProject/Project/Project_Msc/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tumelos_sun_ac_za/Documents/Documents/SACEMA PROJECT/Project/Project_Msc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_73E7C687400C9DDC2165A522FD19852BCDF9DCB7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8494835-7B95-4327-89D6-63B7C3E2DA6F}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_73E7C687400C9DDC2165A522FD19852BCDF9DCB7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C78146F-86FB-4215-A535-F2E8119427DA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -546,8 +546,8 @@
         <v>24</v>
       </c>
       <c r="D2">
-        <f>150000-1</f>
-        <v>149999</v>
+        <f>100000-2</f>
+        <v>99998</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>